<commit_message>
Updated doc to show differences
</commit_message>
<xml_diff>
--- a/signConvention.xlsx
+++ b/signConvention.xlsx
@@ -12,6 +12,107 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+  <si>
+    <t>RSP</t>
+  </si>
+  <si>
+    <t>RSR</t>
+  </si>
+  <si>
+    <t>RSY</t>
+  </si>
+  <si>
+    <t>REP</t>
+  </si>
+  <si>
+    <t>RWY</t>
+  </si>
+  <si>
+    <t>RWR</t>
+  </si>
+  <si>
+    <t>RWP</t>
+  </si>
+  <si>
+    <t>LSP</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LSY</t>
+  </si>
+  <si>
+    <t>LEP</t>
+  </si>
+  <si>
+    <t>LWY</t>
+  </si>
+  <si>
+    <t>LWR</t>
+  </si>
+  <si>
+    <t>LWP</t>
+  </si>
+  <si>
+    <t>HY</t>
+  </si>
+  <si>
+    <t>RHY</t>
+  </si>
+  <si>
+    <t>RHR</t>
+  </si>
+  <si>
+    <t>RHP</t>
+  </si>
+  <si>
+    <t>RKP</t>
+  </si>
+  <si>
+    <t>RAP</t>
+  </si>
+  <si>
+    <t>RAR</t>
+  </si>
+  <si>
+    <t>LHY</t>
+  </si>
+  <si>
+    <t>LHR</t>
+  </si>
+  <si>
+    <t>LHP</t>
+  </si>
+  <si>
+    <t>LKP</t>
+  </si>
+  <si>
+    <t>LAP</t>
+  </si>
+  <si>
+    <t>LAR</t>
+  </si>
+  <si>
+    <t>Joint</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Hubo</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>Sign Convention</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -41,17 +142,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -154,154 +340,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>38272</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>155196</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>287064</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>83236</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="순서도: 자기 디스크 223"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3687080" y="1298196"/>
-          <a:ext cx="248792" cy="499540"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartMagneticDisk">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -2004,8 +2042,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>162669</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>83235</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>108860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -2016,14 +2054,12 @@
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="47" name="직선 연결선 238"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="32" idx="3"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000">
-          <a:off x="3462741" y="2146471"/>
-          <a:ext cx="697471" cy="0"/>
+          <a:off x="1758960" y="1492533"/>
+          <a:ext cx="481346" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3142,160 +3178,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>61688</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>80500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>511429</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>172758</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="순서도: 자기 디스크 253"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="14734889">
-          <a:off x="4402122" y="6474008"/>
-          <a:ext cx="282758" cy="449741"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartMagneticDisk">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:scene3d>
-          <a:camera prst="orthographicFront">
-            <a:rot lat="120728" lon="678112" rev="1192373"/>
-          </a:camera>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
       <xdr:colOff>262636</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>5098</xdr:rowOff>
@@ -4753,253 +4635,6 @@
         <a:xfrm rot="10800000" flipV="1">
           <a:off x="4953001" y="2183422"/>
           <a:ext cx="205155" cy="183174"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>522011</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>421030</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>13817</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="84" name="순서도: 직접 액세스 저장소 275"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3562684" y="874059"/>
-          <a:ext cx="507154" cy="282758"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartMagneticDrum">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>172237</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>23243</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>172237</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>49524</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="85" name="직선 연결선 276"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="5400000">
-          <a:off x="3712654" y="1274634"/>
-          <a:ext cx="216781" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="15875">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>363616</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>62938</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>61688</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>62938</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="직선 화살표 연결선 277"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="4012424" y="1015438"/>
-          <a:ext cx="306206" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5880,56 +5515,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>153100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>73811</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>153100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>156644</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="107" name="직선 화살표 연결선 298"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="5400000">
-          <a:off x="3665241" y="1924978"/>
-          <a:ext cx="273333" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>441181</xdr:colOff>
       <xdr:row>31</xdr:row>
@@ -7696,7 +7281,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>111089</xdr:colOff>
+      <xdr:colOff>61688</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>4804</xdr:rowOff>
     </xdr:from>
@@ -7704,131 +7289,284 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>6015</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>97062</xdr:rowOff>
+      <xdr:rowOff>172758</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 210"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="19007031">
-          <a:off x="2549489" y="5719804"/>
-          <a:ext cx="504526" cy="282758"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="143" name="Group 142"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2500088" y="5719804"/>
+          <a:ext cx="553927" cy="358454"/>
+          <a:chOff x="2510974" y="5719804"/>
+          <a:chExt cx="556648" cy="358454"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>LAR</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="62" name="순서도: 자기 디스크 253"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="14734889">
+            <a:off x="2594466" y="5712008"/>
+            <a:ext cx="282758" cy="449741"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="120728" lon="678112" rev="1192373"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="TextBox 210"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="19007031">
+            <a:off x="2560375" y="5719804"/>
+            <a:ext cx="507247" cy="282758"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+              <a:t>LAR</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -8523,282 +8261,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>531208</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>430616</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4392</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="TextBox 216"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3556796" y="874059"/>
-          <a:ext cx="504526" cy="273333"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>NP</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>40322</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>126920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>287824</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>120937</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="TextBox 217"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="16200000">
-          <a:off x="3512020" y="1428928"/>
-          <a:ext cx="565517" cy="247502"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>NY</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>49841</xdr:colOff>
       <xdr:row>8</xdr:row>
@@ -8927,7 +8389,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>TY</a:t>
+            <a:t>HY</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
         </a:p>
@@ -9485,291 +8947,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>112737</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133181</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>70118</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>10543</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="129" name="Group 128"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm rot="2847760">
-          <a:off x="3315047" y="3598371"/>
-          <a:ext cx="258362" cy="566981"/>
-          <a:chOff x="5160698" y="3767619"/>
-          <a:chExt cx="258362" cy="565516"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="79" name="순서도: 자기 디스크 270"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="5160698" y="3777043"/>
-            <a:ext cx="258362" cy="490114"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartMagneticDisk">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="TextBox 223"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm rot="16200000">
-            <a:off x="5011652" y="3926626"/>
-            <a:ext cx="565516" cy="247502"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-              <a:t>LWR</a:t>
-            </a:r>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -10495,13 +9672,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114395</xdr:colOff>
+      <xdr:colOff>168823</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>69931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>62317</xdr:colOff>
+      <xdr:colOff>116745</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>171618</xdr:rowOff>
     </xdr:to>
@@ -10512,7 +9689,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="114395" y="4260931"/>
+          <a:off x="168823" y="4260931"/>
           <a:ext cx="557522" cy="292187"/>
           <a:chOff x="5016106" y="4370836"/>
           <a:chExt cx="556056" cy="292187"/>
@@ -10780,350 +9957,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>149372</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>23276</xdr:rowOff>
+      <xdr:colOff>70271</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>106754</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91138</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="156" name="Group 155"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm rot="2847760">
-          <a:off x="303682" y="3678966"/>
-          <a:ext cx="258362" cy="566982"/>
-          <a:chOff x="5160698" y="3767619"/>
-          <a:chExt cx="258362" cy="565516"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="157" name="순서도: 자기 디스크 270"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="5160698" y="3777043"/>
-            <a:ext cx="258362" cy="490114"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartMagneticDisk">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="158" name="TextBox 223"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm rot="16200000">
-            <a:off x="5011652" y="3926626"/>
-            <a:ext cx="565516" cy="247502"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-              <a:t>RWR</a:t>
-            </a:r>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6607</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>18747</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>322382</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>18747</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="159" name="직선 화살표 연결선 279"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="2439145" y="5162247"/>
-          <a:ext cx="315775" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>585432</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>175846</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>197830</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>4095</xdr:rowOff>
+      <xdr:colOff>299683</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -11131,9 +9973,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="2409836" y="4366846"/>
-          <a:ext cx="220532" cy="209249"/>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="70271" y="4045417"/>
+          <a:ext cx="229412" cy="213618"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -11165,15 +10007,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>73270</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>27921</xdr:rowOff>
+      <xdr:colOff>576438</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>235765</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168115</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -11181,9 +10023,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="4938347" y="4790421"/>
-          <a:ext cx="162495" cy="162580"/>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3637991" y="3524305"/>
+          <a:ext cx="204107" cy="203999"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -11265,6 +10107,736 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>18747</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>210713</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>20335</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="직선 화살표 연결선 279"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="10800000">
+          <a:off x="0" y="4400247"/>
+          <a:ext cx="210713" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>170545</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114871</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23078</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="144" name="Group 143"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3218545" y="3665124"/>
+          <a:ext cx="553926" cy="358454"/>
+          <a:chOff x="2510974" y="5719804"/>
+          <a:chExt cx="556648" cy="358454"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="145" name="순서도: 자기 디스크 253"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="14734889">
+            <a:off x="2594466" y="5712008"/>
+            <a:ext cx="282758" cy="449741"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="120728" lon="678112" rev="1192373"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="146" name="TextBox 210"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="19007031">
+            <a:off x="2560375" y="5719804"/>
+            <a:ext cx="507247" cy="282758"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+              <a:t>LWR</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>184152</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>100054</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>128479</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>77508</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="147" name="Group 146"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="184152" y="3719554"/>
+          <a:ext cx="553927" cy="358454"/>
+          <a:chOff x="2510974" y="5719804"/>
+          <a:chExt cx="556648" cy="358454"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="148" name="순서도: 자기 디스크 253"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="14734889">
+            <a:off x="2594466" y="5712008"/>
+            <a:ext cx="282758" cy="449741"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="120728" lon="678112" rev="1192373"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="149" name="TextBox 210"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="19007031">
+            <a:off x="2560375" y="5719804"/>
+            <a:ext cx="507247" cy="282758"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+              <a:t>RWR</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>35379</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>187778</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3728357" cy="1642373"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="166" name="TextBox 165"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6131379" y="187778"/>
+          <a:ext cx="3728357" cy="1642373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The sign of the unit vector pointing along the particular joint axis. In the Home position, each body's coordinate system aligns with the global coordinate system.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive pitch = Rotation about +Y Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative pitch = Rotation about -Y Axis (CW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive roll = Rotation about +X Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative roll = Rotation about -X Axis (CW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive yaw = Rotation about +Z Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative yaw = Rotation about -Z Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -20132,6 +19704,104 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3728357" cy="1642373"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="TextBox 111"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="228600"/>
+          <a:ext cx="3728357" cy="1642373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The sign of the unit vector pointing along the particular joint axis. In the Home position, each body's coordinate system aligns with the global coordinate system.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive pitch = Rotation about +Y Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative pitch = Rotation about -Y Axis (CW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive roll = Rotation about +X Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative roll = Rotation about -X Axis (CW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Positive yaw = Rotation about +Z Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Negative yaw = Rotation about -Z Axis (CCW)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -20420,29 +20090,682 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="H1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="8:10">
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="8:10">
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="8:10">
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="8:10">
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="8:10">
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="8:10">
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="8:10">
+      <c r="H7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="8:10">
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="8:10">
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="8:10">
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="8:10">
+      <c r="H11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="8:10">
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="8:10">
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="8:10">
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="8:10">
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="8:10">
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10">
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10">
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10">
+      <c r="H19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10">
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10">
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10">
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10">
+      <c r="H23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10">
+      <c r="H24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10">
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10">
+      <c r="H26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10">
+      <c r="H27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="8:10">
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="8:10">
+      <c r="H29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3:J29">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>NOT($I3=$J3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>($I3=$J3)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="H1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="8:10">
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="8:10">
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="8:10">
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="8:10">
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="8:10">
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="8:10">
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="8:10">
+      <c r="H7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="8:10">
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="8:10">
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="8:10">
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="8:10">
+      <c r="H11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="8:10">
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="8:10">
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="8:10">
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="8:10">
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="8:10">
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10">
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10">
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10">
+      <c r="H19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10">
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10">
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10">
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10">
+      <c r="H23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10">
+      <c r="H24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10">
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10">
+      <c r="H26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10">
+      <c r="H27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="8:10">
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="8:10">
+      <c r="H29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3:J29">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>NOT($I3=$J3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>($I3=$J3)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>